<commit_message>
Load the Excel files into dataframes
</commit_message>
<xml_diff>
--- a/invoices/10001-2023.1.18.xlsx
+++ b/invoices/10001-2023.1.18.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/faf11c8905c299a0/Desktop/картинки для приложения/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serge\PycharmProjects\app4_invoice_generation\invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A199768-F877-4D05-A478-E670D4CB6069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13138399-333C-4545-A5AC-16B842B48F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47E7C708-CB1C-466E-8649-0E93249A4A04}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>product_id</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Product 2</t>
-  </si>
-  <si>
-    <t>Столбец1</t>
   </si>
 </sst>
 </file>
@@ -112,15 +109,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B5C2CE0-5860-4D7E-9975-00AC52562749}" name="Таблица1" displayName="Таблица1" ref="A1:F9" totalsRowShown="0">
-  <autoFilter ref="A1:F9" xr:uid="{9B5C2CE0-5860-4D7E-9975-00AC52562749}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B5C2CE0-5860-4D7E-9975-00AC52562749}" name="Таблица1" displayName="Таблица1" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9" xr:uid="{9B5C2CE0-5860-4D7E-9975-00AC52562749}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{72C92DB7-D822-44A9-B008-9B4FD31CF385}" name="product_id"/>
     <tableColumn id="2" xr3:uid="{3D3F79DE-F12E-4087-8D3D-2B4568530DFA}" name="product_name"/>
     <tableColumn id="3" xr3:uid="{BBAF1796-5346-4BC2-8C88-433B362F6BA0}" name="amount_purchased"/>
     <tableColumn id="4" xr3:uid="{763C1464-E7BB-4026-9524-4D5BF75CE691}" name="price_per_unit"/>
     <tableColumn id="5" xr3:uid="{710B2EB8-64BC-497C-9400-9B2CC56ED71D}" name="total_price"/>
-    <tableColumn id="6" xr3:uid="{FB78768F-C279-4E49-B0D9-3ADAB08987AB}" name="Столбец1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -423,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0A2B00-041D-4F0B-A4E2-602BF4C9F0E0}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,10 +432,9 @@
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,11 +450,8 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7189191</v>
       </c>
@@ -477,7 +469,7 @@
         <v>66.599999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3215674</v>
       </c>

</xml_diff>